<commit_message>
Agregue utilizades a los clientes, agregar y eliminar
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26616"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26809"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DAABE93-9D40-4AF2-99B5-73948F68AEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E397C02A-9588-42DF-9758-9AC0A34EC18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,12 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>cliente</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>tipo</t>
   </si>
   <si>
     <t>telefono</t>
@@ -45,15 +48,24 @@
     <t>monto</t>
   </si>
   <si>
+    <t>anotaciones</t>
+  </si>
+  <si>
     <t>Franco Bonin</t>
   </si>
   <si>
+    <t>CUENTA</t>
+  </si>
+  <si>
     <t>343 5 184 226</t>
   </si>
   <si>
     <t>Peron 70</t>
   </si>
   <si>
+    <t>el mascapito</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lisandro </t>
   </si>
   <si>
@@ -63,6 +75,9 @@
     <t>misione</t>
   </si>
   <si>
+    <t>el mascapoto</t>
+  </si>
+  <si>
     <t>Thiago</t>
   </si>
   <si>
@@ -72,10 +87,16 @@
     <t>churruarin</t>
   </si>
   <si>
+    <t>el capo de la mafia</t>
+  </si>
+  <si>
     <t>juancarlo</t>
   </si>
   <si>
     <t>rocamora3030</t>
+  </si>
+  <si>
+    <t>chupapijas</t>
   </si>
 </sst>
 </file>
@@ -345,22 +366,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -369,83 +390,116 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="12.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
         <v>200000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
         <v>2333232</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
         <v>90000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Primeros cambios despues de usar la apk
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -419,6 +419,9 @@
         <v>monto</v>
       </c>
       <c r="F1" t="str">
+        <v>anotaciones</v>
+      </c>
+      <c r="G1" t="str">
         <v>fechaActualizacion</v>
       </c>
     </row>
@@ -439,12 +442,15 @@
         <v>1001</v>
       </c>
       <c r="F2" t="str">
-        <v>2023-09-06</v>
+        <v>soyyo</v>
+      </c>
+      <c r="G2" t="str">
+        <v>2023-09-07</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>